<commit_message>
full run of addresses complete
</commit_message>
<xml_diff>
--- a/data/input/only_addresses.xlsx
+++ b/data/input/only_addresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizziehealy/Desktop/DSAN_5550/Final Project/Greener_Pastures/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E30F39-778C-3D44-BC55-D92646162D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E062A6FF-5374-B54A-A431-338B9F0E26D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="920" windowWidth="10000" windowHeight="16560" xr2:uid="{515C6852-7ACE-5E4B-B317-CF7BFA03E06A}"/>
+    <workbookView xWindow="13760" yWindow="800" windowWidth="14780" windowHeight="16560" xr2:uid="{515C6852-7ACE-5E4B-B317-CF7BFA03E06A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,21 +341,33 @@
     <t>1383 Cedar Groove Rd</t>
   </si>
   <si>
-    <t>112 Dam View Rd</t>
-  </si>
-  <si>
     <t>100 Walter Mill Lane</t>
   </si>
   <si>
     <t>1236 Hunt Club Lane</t>
   </si>
   <si>
+    <t>727 Iris Ln</t>
+  </si>
+  <si>
+    <t>1343 West Baltimore Pike</t>
+  </si>
+  <si>
+    <t>690 Meadowbrook Lane</t>
+  </si>
+  <si>
+    <t>18 Brookview Rd</t>
+  </si>
+  <si>
+    <t>1 Rose Hill Rd</t>
+  </si>
+  <si>
+    <t>Morton</t>
+  </si>
+  <si>
     <t>1919 Armstrong Ave</t>
   </si>
   <si>
-    <t>Morton</t>
-  </si>
-  <si>
     <t>6 Village Greens Lane</t>
   </si>
   <si>
@@ -500,6 +512,9 @@
     <t>38 Country Village Way</t>
   </si>
   <si>
+    <t>1343 W Baltimore Pike</t>
+  </si>
+  <si>
     <t>643 Darlington Rd</t>
   </si>
   <si>
@@ -578,22 +593,7 @@
     <t>317 S Bobbin Mill Lane</t>
   </si>
   <si>
-    <t>727 Iris Ln</t>
-  </si>
-  <si>
-    <t>1343 West Baltimore Pike</t>
-  </si>
-  <si>
-    <t>690 Meadowbrook Lane</t>
-  </si>
-  <si>
-    <t>55 N Pennell Rd</t>
-  </si>
-  <si>
-    <t>18 Brookview Rd</t>
-  </si>
-  <si>
-    <t>1 Rose Hill Rd</t>
+    <t>55 Pennell Rd</t>
   </si>
 </sst>
 </file>
@@ -636,9 +636,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093C70DC-6579-2E46-B416-E891BA3D477F}">
   <dimension ref="A1:B183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,7 +1140,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1195,7 +1196,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>185</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1334,7 +1335,7 @@
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1363,7 +1364,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>182</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
@@ -1515,7 +1516,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="B67" t="s">
         <v>20</v>
@@ -1755,7 +1756,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="B97" t="s">
         <v>3</v>
@@ -1763,7 +1764,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
         <v>3</v>
@@ -1771,682 +1772,682 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" t="s">
-        <v>105</v>
+      <c r="A100" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" t="s">
-        <v>107</v>
+      <c r="A101" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>108</v>
-      </c>
-      <c r="B102" t="s">
-        <v>107</v>
+      <c r="A102" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>109</v>
-      </c>
-      <c r="B103" t="s">
-        <v>107</v>
+      <c r="A103" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>110</v>
-      </c>
-      <c r="B104" t="s">
-        <v>107</v>
+      <c r="A104" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>111</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="A105" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>112</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="A106" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>113</v>
-      </c>
-      <c r="B107" t="s">
+      <c r="A107" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>114</v>
-      </c>
-      <c r="B108" t="s">
+      <c r="A108" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>115</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="A109" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>116</v>
-      </c>
-      <c r="B110" t="s">
+      <c r="A110" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>117</v>
-      </c>
-      <c r="B111" t="s">
+      <c r="A111" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>118</v>
-      </c>
-      <c r="B112" t="s">
+      <c r="A112" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>119</v>
-      </c>
-      <c r="B113" t="s">
+      <c r="A113" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>120</v>
-      </c>
-      <c r="B114" t="s">
-        <v>121</v>
+      <c r="A114" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>122</v>
-      </c>
-      <c r="B115" t="s">
-        <v>121</v>
+      <c r="A115" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>123</v>
-      </c>
-      <c r="B116" t="s">
-        <v>121</v>
+      <c r="A116" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>124</v>
-      </c>
-      <c r="B117" t="s">
+      <c r="A117" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>126</v>
-      </c>
-      <c r="B118" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>127</v>
-      </c>
-      <c r="B119" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>128</v>
-      </c>
-      <c r="B120" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>129</v>
-      </c>
-      <c r="B121" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>130</v>
-      </c>
-      <c r="B122" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>131</v>
-      </c>
-      <c r="B123" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>132</v>
-      </c>
-      <c r="B124" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>133</v>
-      </c>
-      <c r="B125" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>134</v>
-      </c>
-      <c r="B126" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>135</v>
-      </c>
-      <c r="B127" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>136</v>
-      </c>
-      <c r="B128" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>137</v>
-      </c>
-      <c r="B129" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>137</v>
-      </c>
-      <c r="B130" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>138</v>
-      </c>
-      <c r="B131" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>128</v>
-      </c>
-      <c r="B132" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>139</v>
-      </c>
-      <c r="B133" t="s">
+      <c r="A133" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>140</v>
-      </c>
-      <c r="B134" t="s">
-        <v>121</v>
+      <c r="A134" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>141</v>
-      </c>
-      <c r="B135" t="s">
+      <c r="A135" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>142</v>
-      </c>
-      <c r="B136" t="s">
+      <c r="A136" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>143</v>
-      </c>
-      <c r="B137" t="s">
+      <c r="A137" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>144</v>
-      </c>
-      <c r="B138" t="s">
+      <c r="A138" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>145</v>
-      </c>
-      <c r="B139" t="s">
+      <c r="A139" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>146</v>
-      </c>
-      <c r="B140" t="s">
+      <c r="A140" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>147</v>
-      </c>
-      <c r="B141" t="s">
+      <c r="A141" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>148</v>
-      </c>
-      <c r="B142" t="s">
+      <c r="A142" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>149</v>
-      </c>
-      <c r="B143" t="s">
+      <c r="A143" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>150</v>
-      </c>
-      <c r="B144" t="s">
+      <c r="A144" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>151</v>
-      </c>
-      <c r="B145" t="s">
+      <c r="A145" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>152</v>
-      </c>
-      <c r="B146" t="s">
+      <c r="A146" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>153</v>
-      </c>
-      <c r="B147" t="s">
+      <c r="A147" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="A148" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B148" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>181</v>
-      </c>
-      <c r="B149" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>154</v>
-      </c>
-      <c r="B150" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>155</v>
-      </c>
-      <c r="B151" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>156</v>
-      </c>
-      <c r="B152" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>157</v>
-      </c>
-      <c r="B153" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>159</v>
-      </c>
-      <c r="B154" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>161</v>
-      </c>
-      <c r="B155" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>162</v>
-      </c>
-      <c r="B156" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>163</v>
-      </c>
-      <c r="B157" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>164</v>
-      </c>
-      <c r="B158" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>166</v>
-      </c>
-      <c r="B159" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>167</v>
-      </c>
-      <c r="B160" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>167</v>
-      </c>
-      <c r="B161" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>167</v>
-      </c>
-      <c r="B162" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>167</v>
-      </c>
-      <c r="B163" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>167</v>
-      </c>
-      <c r="B164" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>61</v>
-      </c>
-      <c r="B165" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>61</v>
-      </c>
-      <c r="B166" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>61</v>
-      </c>
-      <c r="B167" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>61</v>
-      </c>
-      <c r="B168" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>61</v>
-      </c>
-      <c r="B169" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>61</v>
-      </c>
-      <c r="B170" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>61</v>
-      </c>
-      <c r="B171" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>61</v>
-      </c>
-      <c r="B172" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>168</v>
-      </c>
-      <c r="B173" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>168</v>
-      </c>
-      <c r="B174" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>169</v>
-      </c>
-      <c r="B175" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>171</v>
-      </c>
-      <c r="B176" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>173</v>
-      </c>
-      <c r="B177" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>174</v>
-      </c>
-      <c r="B178" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>175</v>
-      </c>
-      <c r="B179" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>176</v>
-      </c>
-      <c r="B180" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+      <c r="B182" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B181" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>178</v>
-      </c>
-      <c r="B182" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>179</v>
-      </c>
-      <c r="B183" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>